<commit_message>
pascal excel sheet updated
</commit_message>
<xml_diff>
--- a/Documents/Logboek.xlsx
+++ b/Documents/Logboek.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitWorkshop\Esstelingthegathering\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Avans\jaar 1\1.4\proftaak\Esstelingthegathering\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6452C3-1D56-49F2-B23A-B04959ACF5B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558EC35A-E6B2-4518-8F09-59DAD7F3236F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-13632" windowWidth="24264" windowHeight="13752" activeTab="1" xr2:uid="{9425F2B3-4CB4-4DCB-B8C1-0C6D99F9C061}"/>
+    <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13148" xr2:uid="{9425F2B3-4CB4-4DCB-B8C1-0C6D99F9C061}"/>
   </bookViews>
   <sheets>
     <sheet name="Pascal" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>Activiteit</t>
   </si>
@@ -110,6 +110,21 @@
   </si>
   <si>
     <t>Accounts mogelijk maken</t>
+  </si>
+  <si>
+    <t>nieuw protorype maken zonder mic</t>
+  </si>
+  <si>
+    <t>MQtt onderzoek</t>
+  </si>
+  <si>
+    <t>mqtt op esp32</t>
+  </si>
+  <si>
+    <t>mqtt op anndoid</t>
+  </si>
+  <si>
+    <t>esp32 bugs er uit halen</t>
   </si>
 </sst>
 </file>
@@ -474,16 +489,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61261EF6-4898-445D-AA29-9BD5FBB0A1C0}">
   <dimension ref="B1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -494,7 +509,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -505,7 +520,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -516,7 +531,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -527,7 +542,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -538,15 +553,18 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>15</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>18</v>
       </c>
@@ -557,7 +575,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -568,10 +586,65 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="4:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="D25">
         <f>SUM(D2:D24)</f>
-        <v>5.75</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -584,11 +657,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FC6AB8-5E0F-43ED-92B9-7C5EA2E219C7}">
   <dimension ref="B1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
   </cols>
@@ -667,7 +740,7 @@
       <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="21.88671875" bestFit="1" customWidth="1"/>
   </cols>
@@ -754,7 +827,7 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.88671875" style="1"/>
@@ -823,7 +896,7 @@
       <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Cards added to inventory
Unlocking cards doesnt work yet
</commit_message>
<xml_diff>
--- a/Documents/Logboek.xlsx
+++ b/Documents/Logboek.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitKraken\Esstelingthegathering\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F1B5F1D-D6C5-48B2-B0D6-4BC89DAB08E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED6D6C5-794C-484E-80E5-06DBFAA7A1DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24270" windowHeight="13155" activeTab="3" xr2:uid="{9425F2B3-4CB4-4DCB-B8C1-0C6D99F9C061}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
   <si>
     <t>Activiteit</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t xml:space="preserve">JSON IO </t>
+  </si>
+  <si>
+    <t>Toevoegen card data aan inventory</t>
   </si>
 </sst>
 </file>
@@ -963,7 +966,7 @@
   <dimension ref="B1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,10 +1096,21 @@
         <v>4</v>
       </c>
     </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="1">
+        <v>9</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
     <row r="25" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D25">
         <f>SUM(D2:D24)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
logboek update en rar bestand
</commit_message>
<xml_diff>
--- a/Documents/Logboek.xlsx
+++ b/Documents/Logboek.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\huiswerk\project_1.4\Esstelingthegathering\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B39AD1-7E60-4C37-BAC9-DA1867AF21B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5239420D-1AAF-452C-9E7F-01466DC2A374}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24270" windowHeight="13155" xr2:uid="{9425F2B3-4CB4-4DCB-B8C1-0C6D99F9C061}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24270" windowHeight="13155" activeTab="2" xr2:uid="{9425F2B3-4CB4-4DCB-B8C1-0C6D99F9C061}"/>
   </bookViews>
   <sheets>
     <sheet name="Pascal" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
   <si>
     <t>Activiteit</t>
   </si>
@@ -178,6 +178,12 @@
   </si>
   <si>
     <t xml:space="preserve">JSON IO </t>
+  </si>
+  <si>
+    <t>git managen</t>
+  </si>
+  <si>
+    <t>3t/m9</t>
   </si>
 </sst>
 </file>
@@ -221,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -232,6 +238,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -548,7 +555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61261EF6-4898-445D-AA29-9BD5FBB0A1C0}">
   <dimension ref="B1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -839,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C10B3A5F-D2C3-4516-ABB2-579FD7EEF53A}">
   <dimension ref="B1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,10 +954,21 @@
         <v>2</v>
       </c>
     </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+    </row>
     <row r="26" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D26">
         <f>SUM(D3:D25)</f>
-        <v>22.5</v>
+        <v>24.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>